<commit_message>
OTU -> IFC on website
</commit_message>
<xml_diff>
--- a/docs/eg_data/NHANES/PF/Waist2/Foods/Foods.xlsx
+++ b/docs/eg_data/NHANES/PF/Waist2/Foods/Foods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\Foods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C0416B-0109-4DAB-8575-187599F29699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7351482B-B256-4F99-BA23-98A8AD19A46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28125" yWindow="-3165" windowWidth="22245" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="68">
   <si>
     <t>KCAL</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Alcohol</t>
-  </si>
-  <si>
-    <t>no. of drinks</t>
   </si>
   <si>
     <t>tsp.</t>
@@ -376,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -474,11 +471,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -762,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA68"/>
+  <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,46 +770,46 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1"/>
     </row>
@@ -826,7 +818,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>6</v>
@@ -959,10 +951,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
@@ -1004,7 +996,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1049,13 +1041,13 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D8" s="19">
         <v>0</v>
@@ -1089,7 +1081,7 @@
         <v>*</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P8" s="25"/>
     </row>
@@ -1555,7 +1547,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="D18" s="35">
         <v>7.9189673913043501</v>
@@ -1604,7 +1596,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>5</v>
@@ -1653,13 +1645,13 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>37</v>
-      </c>
       <c r="C20" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="40">
         <v>16.7207820059783</v>
@@ -1705,49 +1697,49 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" t="s">
         <v>61</v>
-      </c>
-      <c r="L23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="H24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N24" s="1"/>
     </row>
@@ -1756,7 +1748,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>6</v>
@@ -1880,10 +1872,10 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
@@ -1922,7 +1914,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
@@ -1964,13 +1956,13 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D30" s="19">
         <v>0</v>
@@ -2004,7 +1996,7 @@
         <v>*</v>
       </c>
       <c r="O30" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -2410,7 +2402,7 @@
         <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>5</v>
@@ -2456,7 +2448,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="D41" s="19">
         <v>7.1735663273710504</v>
@@ -2492,13 +2484,13 @@
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>37</v>
-      </c>
       <c r="C42" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="20">
         <v>16.649647577247698</v>
@@ -2536,7 +2528,7 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D44" s="27"/>
       <c r="S44" s="24"/>
@@ -2551,9 +2543,8 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="27"/>
+        <v>59</v>
+      </c>
       <c r="S45" s="24"/>
       <c r="T45" s="24"/>
       <c r="U45" s="24"/>
@@ -2578,30 +2569,29 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="E47" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="50" t="s">
+      <c r="F47" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F47" s="50" t="s">
-        <v>68</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H47" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="I47" s="48"/>
+        <v>62</v>
+      </c>
+      <c r="H47" t="s">
+        <v>62</v>
+      </c>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
       <c r="S47" s="24"/>
@@ -2626,26 +2616,25 @@
         <v>0.2 (0.6)</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>CONCATENATE(ROUND(E25, 1), " (",ROUND(I25,1),")")</f>
+        <f t="shared" ref="C48:F49" si="4">CONCATENATE(ROUND(E25, 1), " (",ROUND(I25,1),")")</f>
         <v>0.7 (1.1)</v>
       </c>
       <c r="E48" s="3" t="str">
-        <f>CONCATENATE(ROUND(F25, 1), " (",ROUND(J25,1),")")</f>
+        <f t="shared" si="4"/>
         <v>1.1 (1.5)</v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>CONCATENATE(ROUND(G25, 1), " (",ROUND(K25,1),")")</f>
+        <f t="shared" si="4"/>
         <v>1.4 (1.9)</v>
       </c>
-      <c r="G48" s="47" t="str">
-        <f>IF(H48&lt;0.0001,"&lt;0.0001",IF(H48&lt;0.001,"&lt;0.001",IF(H48&lt;0.01,"&lt;0.01",ROUND(H48,3))))</f>
+      <c r="G48" s="3" t="str">
+        <f t="shared" ref="G48:G65" si="5">IF(H48&lt;0.0001,"&lt;0.0001",IF(H48&lt;0.001,"&lt;0.001",IF(H48&lt;0.01,"&lt;0.01",ROUND(H48,3))))</f>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H48" s="49">
-        <f>L25</f>
+      <c r="H48" s="7">
+        <f t="shared" ref="H48:H65" si="6">L25</f>
         <v>1.0498513205627999E-121</v>
       </c>
-      <c r="I48" s="48"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
       <c r="S48" s="24"/>
@@ -2666,30 +2655,29 @@
         <v>6</v>
       </c>
       <c r="C49" s="3" t="str">
-        <f>CONCATENATE(ROUND(D26, 1), " (",ROUND(H26,1),")")</f>
+        <f t="shared" si="4"/>
         <v>5.8 (3.4)</v>
       </c>
       <c r="D49" s="3" t="str">
-        <f>CONCATENATE(ROUND(E26, 1), " (",ROUND(I26,1),")")</f>
+        <f t="shared" si="4"/>
         <v>7 (3.5)</v>
       </c>
       <c r="E49" s="3" t="str">
-        <f>CONCATENATE(ROUND(F26, 1), " (",ROUND(J26,1),")")</f>
+        <f t="shared" si="4"/>
         <v>8.1 (3.7)</v>
       </c>
       <c r="F49" s="3" t="str">
-        <f>CONCATENATE(ROUND(G26, 1), " (",ROUND(K26,1),")")</f>
+        <f t="shared" si="4"/>
         <v>8.9 (4.3)</v>
       </c>
-      <c r="G49" s="47" t="str">
-        <f>IF(H49&lt;0.0001,"&lt;0.0001",IF(H49&lt;0.001,"&lt;0.001",IF(H49&lt;0.01,"&lt;0.01",ROUND(H49,3))))</f>
+      <c r="G49" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H49" s="49">
-        <f>L26</f>
+      <c r="H49" s="7">
+        <f t="shared" si="6"/>
         <v>1.6635055820584701E-65</v>
       </c>
-      <c r="I49" s="48"/>
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
       <c r="S49" s="24"/>
@@ -2710,29 +2698,28 @@
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f>CONCATENATE(ROUND(E27, 1), " (",ROUND(I27,1),")")</f>
+        <f t="shared" ref="D50:F52" si="7">CONCATENATE(ROUND(E27, 1), " (",ROUND(I27,1),")")</f>
         <v>11 (16.2)</v>
       </c>
       <c r="E50" s="3" t="str">
-        <f>CONCATENATE(ROUND(F27, 1), " (",ROUND(J27,1),")")</f>
+        <f t="shared" si="7"/>
         <v>15.5 (19)</v>
       </c>
       <c r="F50" s="3" t="str">
-        <f>CONCATENATE(ROUND(G27, 1), " (",ROUND(K27,1),")")</f>
+        <f t="shared" si="7"/>
         <v>16.9 (20.6)</v>
       </c>
-      <c r="G50" s="47" t="str">
-        <f>IF(H50&lt;0.0001,"&lt;0.0001",IF(H50&lt;0.001,"&lt;0.001",IF(H50&lt;0.01,"&lt;0.01",ROUND(H50,3))))</f>
+      <c r="G50" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H50" s="49">
-        <f>L27</f>
+      <c r="H50" s="7">
+        <f t="shared" si="6"/>
         <v>4.8632115582192202E-105</v>
       </c>
-      <c r="I50" s="48"/>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
       <c r="S50" s="24"/>
@@ -2747,7 +2734,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>31</v>
@@ -2757,26 +2744,25 @@
         <v>0.8 (0.9)</v>
       </c>
       <c r="D51" s="3" t="str">
-        <f>CONCATENATE(ROUND(E28, 1), " (",ROUND(I28,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1 (1)</v>
       </c>
       <c r="E51" s="3" t="str">
-        <f>CONCATENATE(ROUND(F28, 1), " (",ROUND(J28,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1.3 (1.2)</v>
       </c>
       <c r="F51" s="3" t="str">
-        <f>CONCATENATE(ROUND(G28, 1), " (",ROUND(K28,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1.4 (1.4)</v>
       </c>
-      <c r="G51" s="47" t="str">
-        <f>IF(H51&lt;0.0001,"&lt;0.0001",IF(H51&lt;0.001,"&lt;0.001",IF(H51&lt;0.01,"&lt;0.01",ROUND(H51,3))))</f>
+      <c r="G51" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H51" s="49">
-        <f>L28</f>
+      <c r="H51" s="7">
+        <f t="shared" si="6"/>
         <v>1.03578144240093E-29</v>
       </c>
-      <c r="I51" s="48"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
       <c r="S51" s="24"/>
@@ -2791,7 +2777,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>31</v>
@@ -2801,26 +2787,25 @@
         <v>1.4 (0.9)</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f>CONCATENATE(ROUND(E29, 1), " (",ROUND(I29,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1.5 (1)</v>
       </c>
       <c r="E52" s="3" t="str">
-        <f>CONCATENATE(ROUND(F29, 1), " (",ROUND(J29,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1.8 (1)</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f>CONCATENATE(ROUND(G29, 1), " (",ROUND(K29,1),")")</f>
+        <f t="shared" si="7"/>
         <v>1.7 (1)</v>
       </c>
-      <c r="G52" s="47" t="str">
-        <f>IF(H52&lt;0.0001,"&lt;0.0001",IF(H52&lt;0.001,"&lt;0.001",IF(H52&lt;0.01,"&lt;0.01",ROUND(H52,3))))</f>
+      <c r="G52" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H52" s="49">
-        <f>L29</f>
+      <c r="H52" s="7">
+        <f t="shared" si="6"/>
         <v>1.5013294810008501E-16</v>
       </c>
-      <c r="I52" s="48"/>
       <c r="S52" s="24"/>
       <c r="T52" s="24"/>
       <c r="U52" s="24"/>
@@ -2833,37 +2818,37 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C53" s="3" t="str">
-        <f>CONCATENATE(ROUND(D30, 0), " (",ROUND(H30,0),")")</f>
+        <f t="shared" ref="C53:C64" si="8">CONCATENATE(ROUND(D30, 0), " (",ROUND(H30,0),")")</f>
         <v>0 (0)</v>
       </c>
       <c r="D53" s="3" t="str">
-        <f>CONCATENATE(ROUND(E30, 0), " (",ROUND(I30,0),")")</f>
+        <f t="shared" ref="D53:D64" si="9">CONCATENATE(ROUND(E30, 0), " (",ROUND(I30,0),")")</f>
         <v>50 (57)</v>
       </c>
       <c r="E53" s="3" t="str">
-        <f>CONCATENATE(ROUND(F30, 0), " (",ROUND(J30,0),")")</f>
+        <f t="shared" ref="E53:E64" si="10">CONCATENATE(ROUND(F30, 0), " (",ROUND(J30,0),")")</f>
         <v>105 (102)</v>
       </c>
       <c r="F53" s="3" t="str">
-        <f>CONCATENATE(ROUND(G30, 0), " (",ROUND(K30,0),")")</f>
+        <f t="shared" ref="F53:F64" si="11">CONCATENATE(ROUND(G30, 0), " (",ROUND(K30,0),")")</f>
         <v>129 (107)</v>
       </c>
-      <c r="G53" s="47" t="str">
-        <f>IF(H53&lt;0.0001,"&lt;0.0001",IF(H53&lt;0.001,"&lt;0.001",IF(H53&lt;0.01,"&lt;0.01",ROUND(H53,3))))</f>
+      <c r="G53" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H53" s="49">
-        <f>L30</f>
+      <c r="H53" s="7">
+        <f t="shared" si="6"/>
         <v>9.4443410000000005E-68</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
@@ -2885,30 +2870,29 @@
         <v>29</v>
       </c>
       <c r="C54" s="3" t="str">
-        <f>CONCATENATE(ROUND(D31, 0), " (",ROUND(H31,0),")")</f>
+        <f t="shared" si="8"/>
         <v>14 (5)</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f>CONCATENATE(ROUND(E31, 0), " (",ROUND(I31,0),")")</f>
+        <f t="shared" si="9"/>
         <v>16 (5)</v>
       </c>
       <c r="E54" s="3" t="str">
-        <f>CONCATENATE(ROUND(F31, 0), " (",ROUND(J31,0),")")</f>
+        <f t="shared" si="10"/>
         <v>18 (5)</v>
       </c>
       <c r="F54" s="3" t="str">
-        <f>CONCATENATE(ROUND(G31, 0), " (",ROUND(K31,0),")")</f>
+        <f t="shared" si="11"/>
         <v>19 (5)</v>
       </c>
-      <c r="G54" s="47" t="str">
-        <f>IF(H54&lt;0.0001,"&lt;0.0001",IF(H54&lt;0.001,"&lt;0.001",IF(H54&lt;0.01,"&lt;0.01",ROUND(H54,3))))</f>
+      <c r="G54" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H54" s="49">
-        <f>L31</f>
+      <c r="H54" s="7">
+        <f t="shared" si="6"/>
         <v>4.8072698541393398E-98</v>
       </c>
-      <c r="I54" s="48"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
@@ -2920,30 +2904,29 @@
         <v>4</v>
       </c>
       <c r="C55" s="3" t="str">
-        <f>CONCATENATE(ROUND(D32, 0), " (",ROUND(H32,0),")")</f>
+        <f t="shared" si="8"/>
         <v>1954 (720)</v>
       </c>
       <c r="D55" s="3" t="str">
-        <f>CONCATENATE(ROUND(E32, 0), " (",ROUND(I32,0),")")</f>
+        <f t="shared" si="9"/>
         <v>2038 (702)</v>
       </c>
       <c r="E55" s="3" t="str">
-        <f>CONCATENATE(ROUND(F32, 0), " (",ROUND(J32,0),")")</f>
+        <f t="shared" si="10"/>
         <v>2109 (684)</v>
       </c>
       <c r="F55" s="3" t="str">
-        <f>CONCATENATE(ROUND(G32, 0), " (",ROUND(K32,0),")")</f>
+        <f t="shared" si="11"/>
         <v>2225 (743)</v>
       </c>
-      <c r="G55" s="47" t="str">
-        <f>IF(H55&lt;0.0001,"&lt;0.0001",IF(H55&lt;0.001,"&lt;0.001",IF(H55&lt;0.01,"&lt;0.01",ROUND(H55,3))))</f>
+      <c r="G55" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H55" s="49">
-        <f>L32</f>
+      <c r="H55" s="7">
+        <f t="shared" si="6"/>
         <v>4.0303682251243398E-11</v>
       </c>
-      <c r="I55" s="48"/>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -2953,30 +2936,29 @@
         <v>5</v>
       </c>
       <c r="C56" s="9" t="str">
-        <f>CONCATENATE(ROUND(D33, 0), " (",ROUND(H33,0),")")</f>
+        <f t="shared" si="8"/>
         <v>241 (45)</v>
       </c>
       <c r="D56" s="9" t="str">
-        <f>CONCATENATE(ROUND(E33, 0), " (",ROUND(I33,0),")")</f>
+        <f t="shared" si="9"/>
         <v>238 (42)</v>
       </c>
       <c r="E56" s="9" t="str">
-        <f>CONCATENATE(ROUND(F33, 0), " (",ROUND(J33,0),")")</f>
+        <f t="shared" si="10"/>
         <v>240 (46)</v>
       </c>
       <c r="F56" s="9" t="str">
-        <f>CONCATENATE(ROUND(G33, 0), " (",ROUND(K33,0),")")</f>
+        <f t="shared" si="11"/>
         <v>238 (45)</v>
       </c>
       <c r="G56" s="9">
-        <f>IF(H56&lt;0.0001,"&lt;0.0001",IF(H56&lt;0.001,"&lt;0.001",IF(H56&lt;0.01,"&lt;0.01",ROUND(H56,3))))</f>
+        <f t="shared" si="5"/>
         <v>0.30299999999999999</v>
       </c>
-      <c r="H56" s="49">
-        <f>L33</f>
+      <c r="H56" s="7">
+        <f t="shared" si="6"/>
         <v>0.30264775891721102</v>
       </c>
-      <c r="I56" s="48"/>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -2985,31 +2967,30 @@
       <c r="B57" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="47" t="str">
-        <f>CONCATENATE(ROUND(D34, 0), " (",ROUND(H34,0),")")</f>
+      <c r="C57" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>79 (23)</v>
       </c>
-      <c r="D57" s="47" t="str">
-        <f>CONCATENATE(ROUND(E34, 0), " (",ROUND(I34,0),")")</f>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>82 (21)</v>
       </c>
-      <c r="E57" s="47" t="str">
-        <f>CONCATENATE(ROUND(F34, 0), " (",ROUND(J34,0),")")</f>
+      <c r="E57" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>82 (20)</v>
       </c>
-      <c r="F57" s="47" t="str">
-        <f>CONCATENATE(ROUND(G34, 0), " (",ROUND(K34,0),")")</f>
+      <c r="F57" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>82 (20)</v>
       </c>
-      <c r="G57" s="47" t="str">
-        <f>IF(H57&lt;0.0001,"&lt;0.0001",IF(H57&lt;0.001,"&lt;0.001",IF(H57&lt;0.01,"&lt;0.01",ROUND(H57,3))))</f>
+      <c r="G57" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.01</v>
       </c>
-      <c r="H57" s="49">
-        <f>L34</f>
+      <c r="H57" s="7">
+        <f t="shared" si="6"/>
         <v>1.9450024880622199E-3</v>
       </c>
-      <c r="I57" s="48"/>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -3018,31 +2999,30 @@
       <c r="B58" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="47" t="str">
-        <f>CONCATENATE(ROUND(D35, 0), " (",ROUND(H35,0),")")</f>
+      <c r="C58" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>15 (6)</v>
       </c>
-      <c r="D58" s="47" t="str">
-        <f>CONCATENATE(ROUND(E35, 0), " (",ROUND(I35,0),")")</f>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>18 (7)</v>
       </c>
-      <c r="E58" s="47" t="str">
-        <f>CONCATENATE(ROUND(F35, 0), " (",ROUND(J35,0),")")</f>
+      <c r="E58" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>22 (9)</v>
       </c>
-      <c r="F58" s="47" t="str">
-        <f>CONCATENATE(ROUND(G35, 0), " (",ROUND(K35,0),")")</f>
+      <c r="F58" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>24 (9)</v>
       </c>
-      <c r="G58" s="47" t="str">
-        <f>IF(H58&lt;0.0001,"&lt;0.0001",IF(H58&lt;0.001,"&lt;0.001",IF(H58&lt;0.01,"&lt;0.01",ROUND(H58,3))))</f>
+      <c r="G58" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H58" s="49">
-        <f>L35</f>
+      <c r="H58" s="7">
+        <f t="shared" si="6"/>
         <v>6.2283567032546602E-164</v>
       </c>
-      <c r="I58" s="48"/>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -3051,31 +3031,30 @@
       <c r="B59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="47" t="str">
-        <f>CONCATENATE(ROUND(D36, 0), " (",ROUND(H36,0),")")</f>
+      <c r="C59" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>77 (16)</v>
       </c>
-      <c r="D59" s="47" t="str">
-        <f>CONCATENATE(ROUND(E36, 0), " (",ROUND(I36,0),")")</f>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>79 (16)</v>
       </c>
-      <c r="E59" s="47" t="str">
-        <f>CONCATENATE(ROUND(F36, 0), " (",ROUND(J36,0),")")</f>
+      <c r="E59" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>78 (17)</v>
       </c>
-      <c r="F59" s="47" t="str">
-        <f>CONCATENATE(ROUND(G36, 0), " (",ROUND(K36,0),")")</f>
+      <c r="F59" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>81 (18)</v>
       </c>
-      <c r="G59" s="47" t="str">
-        <f>IF(H59&lt;0.0001,"&lt;0.0001",IF(H59&lt;0.001,"&lt;0.001",IF(H59&lt;0.01,"&lt;0.01",ROUND(H59,3))))</f>
+      <c r="G59" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H59" s="49">
-        <f>L36</f>
+      <c r="H59" s="7">
+        <f t="shared" si="6"/>
         <v>6.6575160657740697E-5</v>
       </c>
-      <c r="I59" s="48"/>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -3084,31 +3063,30 @@
       <c r="B60" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="47" t="str">
-        <f>CONCATENATE(ROUND(D37, 0), " (",ROUND(H37,0),")")</f>
+      <c r="C60" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>26 (7)</v>
       </c>
-      <c r="D60" s="47" t="str">
-        <f>CONCATENATE(ROUND(E37, 0), " (",ROUND(I37,0),")")</f>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>25 (7)</v>
       </c>
-      <c r="E60" s="47" t="str">
-        <f>CONCATENATE(ROUND(F37, 0), " (",ROUND(J37,0),")")</f>
+      <c r="E60" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>23 (7)</v>
       </c>
-      <c r="F60" s="47" t="str">
-        <f>CONCATENATE(ROUND(G37, 0), " (",ROUND(K37,0),")")</f>
+      <c r="F60" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>23 (7)</v>
       </c>
-      <c r="G60" s="47" t="str">
-        <f>IF(H60&lt;0.0001,"&lt;0.0001",IF(H60&lt;0.001,"&lt;0.001",IF(H60&lt;0.01,"&lt;0.01",ROUND(H60,3))))</f>
+      <c r="G60" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H60" s="49">
-        <f>L37</f>
+      <c r="H60" s="7">
+        <f t="shared" si="6"/>
         <v>1.2888568912707299E-12</v>
       </c>
-      <c r="I60" s="48"/>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3117,31 +3095,30 @@
       <c r="B61" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="47" t="str">
-        <f>CONCATENATE(ROUND(D38, 0), " (",ROUND(H38,0),")")</f>
+      <c r="C61" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>26 (7)</v>
       </c>
-      <c r="D61" s="47" t="str">
-        <f>CONCATENATE(ROUND(E38, 0), " (",ROUND(I38,0),")")</f>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>28 (7)</v>
       </c>
-      <c r="E61" s="47" t="str">
-        <f>CONCATENATE(ROUND(F38, 0), " (",ROUND(J38,0),")")</f>
+      <c r="E61" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>28 (8)</v>
       </c>
-      <c r="F61" s="47" t="str">
-        <f>CONCATENATE(ROUND(G38, 0), " (",ROUND(K38,0),")")</f>
+      <c r="F61" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>30 (9)</v>
       </c>
-      <c r="G61" s="47" t="str">
-        <f>IF(H61&lt;0.0001,"&lt;0.0001",IF(H61&lt;0.001,"&lt;0.001",IF(H61&lt;0.01,"&lt;0.01",ROUND(H61,3))))</f>
+      <c r="G61" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H61" s="49">
-        <f>L38</f>
+      <c r="H61" s="7">
+        <f t="shared" si="6"/>
         <v>2.1751664148863601E-20</v>
       </c>
-      <c r="I61" s="48"/>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -3150,31 +3127,30 @@
       <c r="B62" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="47" t="str">
-        <f>CONCATENATE(ROUND(D39, 0), " (",ROUND(H39,0),")")</f>
+      <c r="C62" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>17 (6)</v>
       </c>
-      <c r="D62" s="47" t="str">
-        <f>CONCATENATE(ROUND(E39, 0), " (",ROUND(I39,0),")")</f>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>18 (6)</v>
       </c>
-      <c r="E62" s="47" t="str">
-        <f>CONCATENATE(ROUND(F39, 0), " (",ROUND(J39,0),")")</f>
+      <c r="E62" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>19 (6)</v>
       </c>
-      <c r="F62" s="47" t="str">
-        <f>CONCATENATE(ROUND(G39, 0), " (",ROUND(K39,0),")")</f>
+      <c r="F62" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>20 (7)</v>
       </c>
-      <c r="G62" s="47" t="str">
-        <f>IF(H62&lt;0.0001,"&lt;0.0001",IF(H62&lt;0.001,"&lt;0.001",IF(H62&lt;0.01,"&lt;0.01",ROUND(H62,3))))</f>
+      <c r="G62" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H62" s="49">
-        <f>L39</f>
+      <c r="H62" s="7">
+        <f t="shared" si="6"/>
         <v>1.6510316802959001E-19</v>
       </c>
-      <c r="I62" s="48"/>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -3183,109 +3159,94 @@
       <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="47" t="str">
-        <f>CONCATENATE(ROUND(D40, 0), " (",ROUND(H40,0),")")</f>
+      <c r="C63" s="3" t="str">
+        <f t="shared" si="8"/>
         <v>44 (11)</v>
       </c>
-      <c r="D63" s="47" t="str">
-        <f>CONCATENATE(ROUND(E40, 0), " (",ROUND(I40,0),")")</f>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="9"/>
         <v>46 (11)</v>
       </c>
-      <c r="E63" s="47" t="str">
-        <f>CONCATENATE(ROUND(F40, 0), " (",ROUND(J40,0),")")</f>
+      <c r="E63" s="3" t="str">
+        <f t="shared" si="10"/>
         <v>48 (12)</v>
       </c>
-      <c r="F63" s="47" t="str">
-        <f>CONCATENATE(ROUND(G40, 0), " (",ROUND(K40,0),")")</f>
+      <c r="F63" s="3" t="str">
+        <f t="shared" si="11"/>
         <v>50 (14)</v>
       </c>
-      <c r="G63" s="47" t="str">
-        <f>IF(H63&lt;0.0001,"&lt;0.0001",IF(H63&lt;0.001,"&lt;0.001",IF(H63&lt;0.01,"&lt;0.01",ROUND(H63,3))))</f>
+      <c r="G63" s="3" t="str">
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H63" s="49">
-        <f>L40</f>
+      <c r="H63" s="7">
+        <f t="shared" si="6"/>
         <v>3.72793123688149E-26</v>
       </c>
-      <c r="I63" s="48"/>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>33</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>7 (17)</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>6 (14)</v>
+      </c>
+      <c r="E64" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>6 (13)</v>
+      </c>
+      <c r="F64" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>5 (12)</v>
+      </c>
+      <c r="G64" s="3">
+        <f t="shared" si="5"/>
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="6"/>
+        <v>5.7903000498847598E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="47" t="str">
-        <f>CONCATENATE(ROUND(D41, 0), " (",ROUND(H41,0),")")</f>
-        <v>7 (17)</v>
-      </c>
-      <c r="D64" s="47" t="str">
-        <f>CONCATENATE(ROUND(E41, 0), " (",ROUND(I41,0),")")</f>
-        <v>6 (14)</v>
-      </c>
-      <c r="E64" s="47" t="str">
-        <f>CONCATENATE(ROUND(F41, 0), " (",ROUND(J41,0),")")</f>
-        <v>6 (13)</v>
-      </c>
-      <c r="F64" s="47" t="str">
-        <f>CONCATENATE(ROUND(G41, 0), " (",ROUND(K41,0),")")</f>
-        <v>5 (12)</v>
-      </c>
-      <c r="G64" s="47">
-        <f>IF(H64&lt;0.0001,"&lt;0.0001",IF(H64&lt;0.001,"&lt;0.001",IF(H64&lt;0.01,"&lt;0.01",ROUND(H64,3))))</f>
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="H64" s="49">
-        <f>L41</f>
-        <v>5.7903000498847598E-2</v>
-      </c>
-      <c r="I64" s="48"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="C65" s="10" t="str">
-        <f t="shared" ref="C65" si="4">CONCATENATE(ROUND(D42, 0), " (",ROUND(H42,0),")")</f>
+        <f t="shared" ref="C65" si="12">CONCATENATE(ROUND(D42, 0), " (",ROUND(H42,0),")")</f>
         <v>17 (11)</v>
       </c>
       <c r="D65" s="10" t="str">
-        <f t="shared" ref="D65" si="5">CONCATENATE(ROUND(E42, 0), " (",ROUND(I42,0),")")</f>
+        <f t="shared" ref="D65" si="13">CONCATENATE(ROUND(E42, 0), " (",ROUND(I42,0),")")</f>
         <v>14 (8)</v>
       </c>
       <c r="E65" s="10" t="str">
-        <f t="shared" ref="E65" si="6">CONCATENATE(ROUND(F42, 0), " (",ROUND(J42,0),")")</f>
+        <f t="shared" ref="E65" si="14">CONCATENATE(ROUND(F42, 0), " (",ROUND(J42,0),")")</f>
         <v>12 (8)</v>
       </c>
       <c r="F65" s="10" t="str">
-        <f t="shared" ref="F65" si="7">CONCATENATE(ROUND(G42, 0), " (",ROUND(K42,0),")")</f>
+        <f t="shared" ref="F65" si="15">CONCATENATE(ROUND(G42, 0), " (",ROUND(K42,0),")")</f>
         <v>11 (7)</v>
       </c>
       <c r="G65" s="10" t="str">
-        <f>IF(H65&lt;0.0001,"&lt;0.0001",IF(H65&lt;0.001,"&lt;0.001",IF(H65&lt;0.01,"&lt;0.01",ROUND(H65,3))))</f>
+        <f t="shared" si="5"/>
         <v>&lt;0.0001</v>
       </c>
-      <c r="H65" s="49">
-        <f>L42</f>
+      <c r="H65" s="7">
+        <f t="shared" si="6"/>
         <v>3.7557936039960502E-36</v>
       </c>
-      <c r="I65" s="48"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H68" s="48"/>
-      <c r="I68" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3294,7 +3255,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{B8630206-E012-404C-8CB6-5FB7A7C01591}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{07FC28DC-BEA2-49E7-857D-B5E552A93230}">
           <x14:colorSeries theme="5"/>
           <x14:colorNegative theme="6"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3305,76 +3266,12 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!D3:G3</xm:f>
-              <xm:sqref>N3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D4:G4</xm:f>
-              <xm:sqref>N4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D5:G5</xm:f>
-              <xm:sqref>N5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D6:G6</xm:f>
-              <xm:sqref>N6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D7:G7</xm:f>
-              <xm:sqref>N7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D8:G8</xm:f>
-              <xm:sqref>N8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D9:G9</xm:f>
-              <xm:sqref>N9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D10:G10</xm:f>
-              <xm:sqref>N10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D11:G11</xm:f>
-              <xm:sqref>N11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D12:G12</xm:f>
-              <xm:sqref>N12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D13:G13</xm:f>
-              <xm:sqref>N13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D14:G14</xm:f>
-              <xm:sqref>N14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D15:G15</xm:f>
-              <xm:sqref>N15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D16:G16</xm:f>
-              <xm:sqref>N16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D17:G17</xm:f>
-              <xm:sqref>N17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D18:G18</xm:f>
-              <xm:sqref>N18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D19:G19</xm:f>
-              <xm:sqref>N19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D20:G20</xm:f>
-              <xm:sqref>N20</xm:sqref>
+              <xm:f>Sheet1!D31:G31</xm:f>
+              <xm:sqref>N31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D32:G32</xm:f>
+              <xm:sqref>N32</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -3454,7 +3351,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{07FC28DC-BEA2-49E7-857D-B5E552A93230}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{B8630206-E012-404C-8CB6-5FB7A7C01591}">
           <x14:colorSeries theme="5"/>
           <x14:colorNegative theme="6"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3465,12 +3362,76 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!D31:G31</xm:f>
-              <xm:sqref>N31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!D32:G32</xm:f>
-              <xm:sqref>N32</xm:sqref>
+              <xm:f>Sheet1!D3:G3</xm:f>
+              <xm:sqref>N3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D4:G4</xm:f>
+              <xm:sqref>N4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D5:G5</xm:f>
+              <xm:sqref>N5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D6:G6</xm:f>
+              <xm:sqref>N6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D7:G7</xm:f>
+              <xm:sqref>N7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D8:G8</xm:f>
+              <xm:sqref>N8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D9:G9</xm:f>
+              <xm:sqref>N9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D10:G10</xm:f>
+              <xm:sqref>N10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D11:G11</xm:f>
+              <xm:sqref>N11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D12:G12</xm:f>
+              <xm:sqref>N12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D13:G13</xm:f>
+              <xm:sqref>N13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D14:G14</xm:f>
+              <xm:sqref>N14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D15:G15</xm:f>
+              <xm:sqref>N15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D16:G16</xm:f>
+              <xm:sqref>N16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D17:G17</xm:f>
+              <xm:sqref>N17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D18:G18</xm:f>
+              <xm:sqref>N18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D19:G19</xm:f>
+              <xm:sqref>N19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D20:G20</xm:f>
+              <xm:sqref>N20</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>